<commit_message>
fix missing events for outbound
</commit_message>
<xml_diff>
--- a/resources/samples/SampleMappings_20.xlsx
+++ b/resources/samples/SampleMappings_20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ck/work/git/cumulocity-dynamic-mapper/resources/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E01072-1B19-244C-AFD8-891A8ED02FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0ADA92-C8C2-C04C-A454-F2C2758F2A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7800" yWindow="-24100" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1691,8 +1691,8 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>